<commit_message>
implemented till file and table
</commit_message>
<xml_diff>
--- a/Data_validation_input.xlsx
+++ b/Data_validation_input.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Input" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SQL-Snowflake Datatype Mapping" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="57">
   <si>
     <t xml:space="preserve">S No.</t>
   </si>
@@ -62,6 +63,126 @@
     <t xml:space="preserve">dbo</t>
   </si>
   <si>
+    <t xml:space="preserve">user_Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\Sampath.Gudisa\Downloads\MOCK_DATA.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQLServer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snowflake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bigint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOLEAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">money</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smallint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smallmoney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tinyint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLOAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIMESTAMP_NTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetimeoffset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIMESTAMP_LTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smalldatetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">char</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ntext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nvarchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BINARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varbinary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Product</t>
   </si>
   <si>
@@ -72,120 +193,6 @@
   </si>
   <si>
     <t xml:space="preserve">candidates_changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQLServer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snowflake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bigint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOOLEAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">money</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numeric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smallint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smallmoney</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tinyint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLOAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">real</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datetime2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIMESTAMP_NTZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datetimeoffset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIMESTAMP_LTZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smalldatetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">char</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEXT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ntext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nvarchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">binary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BINARY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varbinary</t>
   </si>
 </sst>
 </file>
@@ -324,7 +331,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -345,14 +352,14 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -363,6 +370,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -444,8 +455,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -497,82 +508,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -595,7 +572,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="I2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -607,320 +584,504 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="1" sqref="I2 I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="46.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="45.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="47.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="30.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="8.6"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
handled nulls and encoding
</commit_message>
<xml_diff>
--- a/Data_validation_input.xlsx
+++ b/Data_validation_input.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Input" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SQL-Snowflake Datatype Mapping" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SampleScenarios_template" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -360,12 +360,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -455,8 +455,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -531,33 +531,22 @@
       <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -905,7 +894,7 @@
       <c r="B27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -925,8 +914,8 @@
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1002,7 +991,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
+      <c r="A3" s="8" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1014,22 +1003,22 @@
       <c r="D3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="8" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1041,22 +1030,22 @@
       <c r="D4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="8" t="n">
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1073,7 +1062,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+      <c r="A6" s="8" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1085,11 +1074,12 @@
       <c r="D6" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I7" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="I7" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>